<commit_message>
Added encoding for utf-8
</commit_message>
<xml_diff>
--- a/text_generator/templates/new_templates.xlsx
+++ b/text_generator/templates/new_templates.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="145">
   <si>
     <t>Subject</t>
   </si>
@@ -204,148 +204,253 @@
     <t>, офіс якої розташований за адресою ?address</t>
   </si>
   <si>
-    <t>Студент</t>
+    <t>Студента</t>
+  </si>
+  <si>
+    <t>запросили</t>
+  </si>
+  <si>
+    <t>на інтернатуру</t>
+  </si>
+  <si>
+    <t>в ?org_name</t>
+  </si>
+  <si>
+    <t>Я</t>
+  </si>
+  <si>
+    <t>приїхав</t>
+  </si>
+  <si>
+    <t>на подію</t>
+  </si>
+  <si>
+    <t>від компанії ?org_name</t>
+  </si>
+  <si>
+    <t>Акціонер</t>
+  </si>
+  <si>
+    <t>зробив</t>
+  </si>
+  <si>
+    <t>великий прибуток</t>
+  </si>
+  <si>
+    <t>, продавши акції компанії ?org_name</t>
+  </si>
+  <si>
+    <t>Бухгалтер</t>
+  </si>
+  <si>
+    <t>помилився</t>
+  </si>
+  <si>
+    <t>в розрахунках</t>
+  </si>
+  <si>
+    <t>заробітної плати працівників компанії ?org_name</t>
+  </si>
+  <si>
+    <t>Водій</t>
+  </si>
+  <si>
+    <t>вчасно</t>
+  </si>
+  <si>
+    <t>за директором ?org_name</t>
+  </si>
+  <si>
+    <t>Президент</t>
+  </si>
+  <si>
+    <t>прийняв</t>
+  </si>
+  <si>
+    <t>новий закон</t>
+  </si>
+  <si>
+    <t>, який накладає певні обмеження на діяльніть ?org_name</t>
+  </si>
+  <si>
+    <t>Парламент</t>
+  </si>
+  <si>
+    <t>запропонував</t>
+  </si>
+  <si>
+    <t>нові правила</t>
+  </si>
+  <si>
+    <t>, щодо регулювання дыяльності ?org_name</t>
+  </si>
+  <si>
+    <t>Касир</t>
+  </si>
+  <si>
+    <t>працює</t>
+  </si>
+  <si>
+    <t>в магазині</t>
+  </si>
+  <si>
+    <t>, власником якого є ?org_name</t>
+  </si>
+  <si>
+    <t>, який знаходиться за адресою ?address</t>
+  </si>
+  <si>
+    <t>співпрацює</t>
+  </si>
+  <si>
+    <t>з компанією</t>
+  </si>
+  <si>
+    <t>?org_name</t>
+  </si>
+  <si>
+    <t>, яка зареєстрована за адресою ?address</t>
+  </si>
+  <si>
+    <t>Лікар</t>
+  </si>
+  <si>
+    <t>вилікував</t>
+  </si>
+  <si>
+    <t>від тяжкої хвороби</t>
+  </si>
+  <si>
+    <t>працівника компанії ?org_name</t>
+  </si>
+  <si>
+    <t>, який проживає за адресою ?address</t>
+  </si>
+  <si>
+    <t>Трейдер</t>
+  </si>
+  <si>
+    <t>втратив</t>
+  </si>
+  <si>
+    <t>кошти</t>
+  </si>
+  <si>
+    <t>, бо невчасно продав акції компанії ?org_name</t>
+  </si>
+  <si>
+    <t>Перекладач</t>
+  </si>
+  <si>
+    <t>звільнився</t>
+  </si>
+  <si>
+    <t>з роботи</t>
+  </si>
+  <si>
+    <t>, бо компанія ?org_name майже банкрут</t>
+  </si>
+  <si>
+    <t>Він</t>
+  </si>
+  <si>
+    <t>жив</t>
+  </si>
+  <si>
+    <t>в офісі</t>
+  </si>
+  <si>
+    <t>компанії ?org_name</t>
+  </si>
+  <si>
+    <t>Вона</t>
+  </si>
+  <si>
+    <t>привезла</t>
+  </si>
+  <si>
+    <t>документи</t>
+  </si>
+  <si>
+    <t>в офіс компанії ?org_name</t>
+  </si>
+  <si>
+    <t>Вони</t>
+  </si>
+  <si>
+    <t>збудували</t>
+  </si>
+  <si>
+    <t>офіс</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> компанії ?org_name</t>
+  </si>
+  <si>
+    <t>Компанія</t>
+  </si>
+  <si>
+    <t>уклала</t>
+  </si>
+  <si>
+    <t>угоду</t>
+  </si>
+  <si>
+    <t>Таксист</t>
+  </si>
+  <si>
+    <t>підвіз</t>
+  </si>
+  <si>
+    <t>людину</t>
+  </si>
+  <si>
+    <t>, яка працює в ?org_name</t>
+  </si>
+  <si>
+    <t>Банкір</t>
+  </si>
+  <si>
+    <t>надав</t>
+  </si>
+  <si>
+    <t>фінансові послуги</t>
+  </si>
+  <si>
+    <t>Військовий</t>
   </si>
   <si>
     <t>отримав</t>
   </si>
   <si>
-    <t>запрошення</t>
-  </si>
-  <si>
-    <t>на інтернатуру в ?org_name</t>
-  </si>
-  <si>
-    <t>Я</t>
-  </si>
-  <si>
-    <t>приїхав</t>
-  </si>
-  <si>
-    <t>на подію</t>
-  </si>
-  <si>
-    <t>від компанії ?org_name</t>
-  </si>
-  <si>
-    <t>Акціонер</t>
-  </si>
-  <si>
-    <t>зробив</t>
-  </si>
-  <si>
-    <t>великий прибуток</t>
-  </si>
-  <si>
-    <t>, продавши акції компанії ?org_name</t>
-  </si>
-  <si>
-    <t>Бухгалтер</t>
-  </si>
-  <si>
-    <t>помилку</t>
-  </si>
-  <si>
-    <t>в розрахунках заробітної плати працівників компанії ?org_name</t>
-  </si>
-  <si>
-    <t>Водій</t>
-  </si>
-  <si>
-    <t>вчасно</t>
-  </si>
-  <si>
-    <t>за директором ?org_name</t>
-  </si>
-  <si>
-    <t>Президент</t>
-  </si>
-  <si>
-    <t>прийняв</t>
-  </si>
-  <si>
-    <t>новий закон</t>
-  </si>
-  <si>
-    <t>, який накладає певні обмеження на діяльніть ?org_name</t>
-  </si>
-  <si>
-    <t>Парламент</t>
-  </si>
-  <si>
-    <t>запропонував</t>
-  </si>
-  <si>
-    <t>нові правила</t>
-  </si>
-  <si>
-    <t>, щодо регулювання дыяльності ?org_name</t>
-  </si>
-  <si>
-    <t>Касир</t>
-  </si>
-  <si>
-    <t>працює</t>
-  </si>
-  <si>
-    <t>в магазині</t>
-  </si>
-  <si>
-    <t>, власником якого є ?org_name</t>
-  </si>
-  <si>
-    <t>, який знаходиться за адресою ?address</t>
-  </si>
-  <si>
-    <t>співпрацює</t>
-  </si>
-  <si>
-    <t>з компанією</t>
-  </si>
-  <si>
-    <t>?org_name</t>
-  </si>
-  <si>
-    <t>, яка зареєстрована за адресою ?address</t>
-  </si>
-  <si>
-    <t>Лікар</t>
-  </si>
-  <si>
-    <t>вилікував</t>
-  </si>
-  <si>
-    <t>від тяжкої хвороби</t>
-  </si>
-  <si>
-    <t>працівника компанії ?org_name</t>
-  </si>
-  <si>
-    <t>, який проживає за адресою ?address</t>
-  </si>
-  <si>
-    <t>Трейдер</t>
-  </si>
-  <si>
-    <t>втратив</t>
-  </si>
-  <si>
-    <t>кошти</t>
-  </si>
-  <si>
-    <t>, бо невчасно продав акції компанії ?org_name</t>
-  </si>
-  <si>
-    <t>Перекладач</t>
-  </si>
-  <si>
-    <t>звільнився</t>
-  </si>
-  <si>
-    <t>з роботи</t>
-  </si>
-  <si>
-    <t>, бо компанія ?org_name майже банкрут</t>
+    <t>фінансову допомогу</t>
+  </si>
+  <si>
+    <t>придбав</t>
+  </si>
+  <si>
+    <t>частину</t>
+  </si>
+  <si>
+    <t>Літак</t>
+  </si>
+  <si>
+    <t>нажелить</t>
+  </si>
+  <si>
+    <t>компанії</t>
+  </si>
+  <si>
+    <t>Бізнесмен</t>
+  </si>
+  <si>
+    <t>продав</t>
+  </si>
+  <si>
+    <t>чатину</t>
+  </si>
+  <si>
+    <t>акцій компанії ?org_name</t>
   </si>
 </sst>
 </file>
@@ -908,27 +1013,27 @@
         <v>74</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="19" ht="15.75" customHeight="1">
       <c r="A19" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>67</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>26</v>
@@ -936,47 +1041,47 @@
     </row>
     <row r="20" ht="15.75" customHeight="1">
       <c r="A20" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1">
       <c r="A21" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="22" ht="15.75" customHeight="1">
       <c r="A22" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="23" ht="15.75" customHeight="1">
@@ -984,73 +1089,218 @@
         <v>5</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="24" ht="15.75" customHeight="1">
       <c r="A24" s="2" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="25" ht="15.75" customHeight="1">
       <c r="A25" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="26" ht="15.75" customHeight="1">
       <c r="A26" s="2" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="27" ht="15.75" customHeight="1"/>
-    <row r="28" ht="15.75" customHeight="1"/>
-    <row r="29" ht="15.75" customHeight="1"/>
-    <row r="30" ht="15.75" customHeight="1"/>
-    <row r="31" ht="15.75" customHeight="1"/>
-    <row r="32" ht="15.75" customHeight="1"/>
-    <row r="33" ht="15.75" customHeight="1"/>
-    <row r="34" ht="15.75" customHeight="1"/>
-    <row r="35" ht="15.75" customHeight="1"/>
-    <row r="36" ht="15.75" customHeight="1"/>
+        <v>110</v>
+      </c>
+    </row>
+    <row r="27" ht="15.75" customHeight="1">
+      <c r="A27" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" ht="15.75" customHeight="1">
+      <c r="A28" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="29" ht="15.75" customHeight="1">
+      <c r="A29" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="30" ht="15.75" customHeight="1">
+      <c r="A30" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" ht="15.75" customHeight="1">
+      <c r="A31" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="32" ht="15.75" customHeight="1">
+      <c r="A32" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="33" ht="15.75" customHeight="1">
+      <c r="A33" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="34" ht="15.75" customHeight="1">
+      <c r="A34" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="35" ht="15.75" customHeight="1">
+      <c r="A35" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="36" ht="15.75" customHeight="1">
+      <c r="A36" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>144</v>
+      </c>
+    </row>
     <row r="37" ht="15.75" customHeight="1"/>
     <row r="38" ht="15.75" customHeight="1"/>
     <row r="39" ht="15.75" customHeight="1"/>

</xml_diff>